<commit_message>
siguen modificaciones en salidas de campos
</commit_message>
<xml_diff>
--- a/tabla_b.xlsx
+++ b/tabla_b.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>SUMINISTRO</t>
   </si>
@@ -27,136 +27,73 @@
     <t>NOMBRES</t>
   </si>
   <si>
-    <t>NUMEROFICHA</t>
+    <t>NUMEROFICHA_x</t>
+  </si>
+  <si>
+    <t>NUMEROFICHA_y</t>
   </si>
   <si>
     <t>ROSA JULIA GARCIA CARHUAYO</t>
   </si>
   <si>
-    <t>332076ROSA JULIA GARCIA CARHUAYO</t>
-  </si>
-  <si>
-    <t>332074ROSA JULIA GARCIA CARHUAYO</t>
-  </si>
-  <si>
     <t>ISABEL GALVAN CANTORAL</t>
   </si>
   <si>
-    <t>332079ISABEL GALVAN CANTORAL</t>
-  </si>
-  <si>
     <t>CLEMENTINA LOVERA VDA. DE FLORES</t>
   </si>
   <si>
-    <t>269811CLEMENTINA LOVERA VDA. DE FLORES</t>
-  </si>
-  <si>
     <t>MARIA M. TATAJE M.</t>
   </si>
   <si>
-    <t>332078MARIA M. TATAJE M.</t>
-  </si>
-  <si>
     <t>PEDRO JULIO ESCATE MUÑANTE</t>
   </si>
   <si>
-    <t>332077PEDRO JULIO ESCATE MUÑANTE</t>
-  </si>
-  <si>
     <t>ISABEL LEVANO D.</t>
   </si>
   <si>
-    <t>332075ISABEL LEVANO D.</t>
-  </si>
-  <si>
     <t>NILTON FELIPE HUAYLLA ZEGARRA</t>
   </si>
   <si>
-    <t>332073NILTON FELIPE HUAYLLA ZEGARRA</t>
-  </si>
-  <si>
     <t>PEDRO MARTINEZ</t>
   </si>
   <si>
-    <t>332072PEDRO MARTINEZ</t>
-  </si>
-  <si>
     <t>MARIA HAYDEE MUÑOZ DE MONTERREY</t>
   </si>
   <si>
-    <t>332071MARIA HAYDEE MUÑOZ DE MONTERREY</t>
-  </si>
-  <si>
     <t>ROSE MARY GONZALES DE GASTELU</t>
   </si>
   <si>
-    <t>332070ROSE MARY GONZALES DE GASTELU</t>
-  </si>
-  <si>
     <t>INVERSIONES EL CATADOR S.A.C.</t>
   </si>
   <si>
-    <t>332069INVERSIONES EL CATADOR S.A.C.</t>
-  </si>
-  <si>
     <t>LEONCIO GONZALES M.</t>
   </si>
   <si>
-    <t>332068LEONCIO GONZALES M.</t>
-  </si>
-  <si>
     <t>JORGE CARRASCO P.</t>
   </si>
   <si>
-    <t>332067JORGE CARRASCO P.</t>
-  </si>
-  <si>
     <t>CRISTEL ROXANA CARRASCO GONZALES</t>
   </si>
   <si>
-    <t>332066CRISTEL ROXANA CARRASCO GONZALES</t>
-  </si>
-  <si>
     <t>REST.CAMP.LA OLLA DE JUANITA E.I.R.L.</t>
   </si>
   <si>
-    <t>332065REST.CAMP.LA OLLA DE JUANITA E.I.R.L.</t>
-  </si>
-  <si>
     <t>ANGELA DE PEÑA</t>
   </si>
   <si>
-    <t>332064ANGELA DE PEÑA</t>
-  </si>
-  <si>
     <t>JUANA ROSA PEÑA LEVANO</t>
   </si>
   <si>
-    <t>332063JUANA ROSA PEÑA LEVANO</t>
-  </si>
-  <si>
     <t>PABLO MAURO LOPEZ MAYURI</t>
   </si>
   <si>
-    <t>332062PABLO MAURO LOPEZ MAYURI</t>
-  </si>
-  <si>
     <t>LA CAPILLA DE TRES ESQUINAS</t>
   </si>
   <si>
-    <t>332061LA CAPILLA DE TRES ESQUINAS</t>
-  </si>
-  <si>
     <t>VERONICA SABINA VASQUEZ MOQUILLAZA</t>
   </si>
   <si>
-    <t>332060VERONICA SABINA VASQUEZ MOQUILLAZA</t>
-  </si>
-  <si>
     <t>JUAN CARLOS ROMANI QUISPE</t>
-  </si>
-  <si>
-    <t>268940JUAN CARLOS ROMANI QUISPE</t>
   </si>
 </sst>
 </file>
@@ -519,20 +456,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,269 +477,316 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101067264</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>332076</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>101067264</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>332074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>101067264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>332076</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>101067264</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>332074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>101074942</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>101074942</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D6">
+        <v>332079</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>101028629</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D7">
+        <v>269811</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>101028722</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>101028629</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D8">
+        <v>332078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>101028737</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D9">
+        <v>332077</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>101028727</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>101028722</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D10">
+        <v>332075</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>101067264</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>332076</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>101067264</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>332074</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>101067264</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>332076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>101067264</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>332074</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>101091029</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D15">
+        <v>332073</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>101028603</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>101028737</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D16">
+        <v>332072</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>101055755</v>
+      </c>
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D17">
+        <v>332071</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>101056432</v>
+      </c>
+      <c r="B18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>101028727</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D18">
+        <v>332070</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>700028026</v>
+      </c>
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D19">
+        <v>332069</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>101027103</v>
+      </c>
+      <c r="B20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>101067264</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>101067264</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>101091029</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D20">
+        <v>332068</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>101027105</v>
+      </c>
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D21">
+        <v>332067</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>101064641</v>
+      </c>
+      <c r="B22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>101028603</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D22">
+        <v>332066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>101070480</v>
+      </c>
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D23">
+        <v>332065</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>101027100</v>
+      </c>
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>101055755</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D24">
+        <v>332064</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>101062381</v>
+      </c>
+      <c r="B25" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D25">
+        <v>332063</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>101053333</v>
+      </c>
+      <c r="B26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>101056432</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D26">
+        <v>332062</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>101074948</v>
+      </c>
+      <c r="B27" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D27">
+        <v>332061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>101061521</v>
+      </c>
+      <c r="B28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>700028026</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D28">
+        <v>332060</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>700008306</v>
+      </c>
+      <c r="B29" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>101027103</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>101027105</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>101064641</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>101070480</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>101027100</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>101062381</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>101053333</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>101074948</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>101061521</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>700008306</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
+      <c r="D29">
+        <v>268940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>